<commit_message>
[FEAT] added function overwritePurchaseReport(), to overwrite purchase record data in 'historicoCompras.json'
</commit_message>
<xml_diff>
--- a/src/data/relatorios/xlsx/relatorio.xlsx
+++ b/src/data/relatorios/xlsx/relatorio.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Relatório Compra 12-03-2025" sheetId="1" r:id="rId1"/>
+    <sheet name="Relatório Compra 13-03-2025" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -445,7 +445,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -454,245 +454,1237 @@
         <v>20</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="H2">
-        <v>6.33</v>
+        <v>8.7</v>
       </c>
       <c r="I2">
         <v>0.5818</v>
       </c>
       <c r="J2">
-        <v>80</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B3" t="str">
-        <v>LIMAO TAITI</v>
+        <v>ABACAXI PEROLA</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D3">
-        <v>80</v>
+        <v>7.5</v>
       </c>
       <c r="E3">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G3">
-        <v>3.64</v>
+        <v>7.5</v>
       </c>
       <c r="H3">
-        <v>5.75</v>
+        <v>11.85</v>
       </c>
       <c r="I3">
         <v>0.58</v>
       </c>
       <c r="J3">
-        <v>80</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="B4" t="str">
-        <v>SALSA</v>
+        <v>BANANA NANICA</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
+        <v>65</v>
+      </c>
+      <c r="E4">
         <v>20</v>
       </c>
-      <c r="E4">
-        <v>19</v>
-      </c>
       <c r="F4">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="G4">
-        <v>1.05</v>
+        <v>3.25</v>
       </c>
       <c r="H4">
-        <v>1.66</v>
+        <v>5.13</v>
       </c>
       <c r="I4">
         <v>0.58</v>
       </c>
       <c r="J4">
-        <v>20</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="B5" t="str">
-        <v>ABOBORA SECA</v>
+        <v>BANANA PRATA</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="G5">
-        <v>80</v>
+        <v>4.25</v>
       </c>
       <c r="H5">
-        <v>126.4</v>
+        <v>6.71</v>
       </c>
       <c r="I5">
-        <v>0.58</v>
+        <v>0.5788</v>
       </c>
       <c r="J5">
-        <v>80</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B6" t="str">
-        <v>ABACAXI PEROLA</v>
+        <v>COCO SECO</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G6">
-        <v>80</v>
+        <v>5.5</v>
       </c>
       <c r="H6">
-        <v>126.4</v>
+        <v>8.69</v>
       </c>
       <c r="I6">
         <v>0.58</v>
       </c>
       <c r="J6">
-        <v>160</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B7" t="str">
-        <v>MACA GALA</v>
+        <v>GOIABA VERMELHA</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="E7">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F7">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="G7">
-        <v>4.44</v>
+        <v>5</v>
       </c>
       <c r="H7">
-        <v>7.02</v>
+        <v>7.9</v>
       </c>
       <c r="I7">
-        <v>0.5798</v>
+        <v>0.58</v>
       </c>
       <c r="J7">
-        <v>160</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="B8" t="str">
-        <v>BERINJELA</v>
+        <v>KIWI AMARELO</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E8">
         <v>10</v>
       </c>
       <c r="F8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H8">
-        <v>13.6</v>
+        <v>11.06</v>
       </c>
       <c r="I8">
-        <v>0.7</v>
+        <v>0.58</v>
       </c>
       <c r="J8">
-        <v>160</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B9" t="str">
-        <v>ALFACE CRESPA</v>
+        <v>LARANJA PERA</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9">
+        <v>110</v>
+      </c>
+      <c r="E9">
+        <v>22</v>
+      </c>
+      <c r="F9">
+        <v>44</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>7.9</v>
+      </c>
+      <c r="I9">
+        <v>0.58</v>
+      </c>
+      <c r="J9">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>21</v>
+      </c>
+      <c r="B10" t="str">
+        <v>LIMAO TAITI</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+      <c r="E10">
+        <v>22</v>
+      </c>
+      <c r="F10">
+        <v>22</v>
+      </c>
+      <c r="G10">
+        <v>2.27</v>
+      </c>
+      <c r="H10">
+        <v>3.59</v>
+      </c>
+      <c r="I10">
+        <v>0.58</v>
+      </c>
+      <c r="J10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>22</v>
+      </c>
+      <c r="B11" t="str">
+        <v>MACA ARGENTINA</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>140</v>
+      </c>
+      <c r="E11">
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <v>18</v>
+      </c>
+      <c r="G11">
+        <v>7.78</v>
+      </c>
+      <c r="H11">
+        <v>12.29</v>
+      </c>
+      <c r="I11">
+        <v>0.5797</v>
+      </c>
+      <c r="J11">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>23</v>
+      </c>
+      <c r="B12" t="str">
+        <v>MACA GALA</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>150</v>
+      </c>
+      <c r="E12">
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>18</v>
+      </c>
+      <c r="G12">
+        <v>8.33</v>
+      </c>
+      <c r="H12">
+        <v>13.17</v>
+      </c>
+      <c r="I12">
+        <v>0.5798</v>
+      </c>
+      <c r="J12">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="str">
+        <v>MAMAO PAPAIA</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>45</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>90</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>4.74</v>
+      </c>
+      <c r="I13">
+        <v>0.58</v>
+      </c>
+      <c r="J13">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>25</v>
+      </c>
+      <c r="B14" t="str">
+        <v>MANGA PALMER</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>85</v>
+      </c>
+      <c r="E14">
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>34</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>7.9</v>
+      </c>
+      <c r="I14">
+        <v>0.58</v>
+      </c>
+      <c r="J14">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>26</v>
+      </c>
+      <c r="B15" t="str">
+        <v>MANGA TOMMY</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>130</v>
+      </c>
+      <c r="E15">
+        <v>17</v>
+      </c>
+      <c r="F15">
+        <v>17</v>
+      </c>
+      <c r="G15">
+        <v>7.65</v>
+      </c>
+      <c r="H15">
+        <v>12.08</v>
+      </c>
+      <c r="I15">
+        <v>0.58</v>
+      </c>
+      <c r="J15">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>1393</v>
+      </c>
+      <c r="B16" t="str">
+        <v>AMEIXA FORTUNA</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>110</v>
+      </c>
+      <c r="E16">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>12.22</v>
+      </c>
+      <c r="H16">
+        <v>19.31</v>
+      </c>
+      <c r="I16">
+        <v>0.5802</v>
+      </c>
+      <c r="J16">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>27</v>
+      </c>
+      <c r="B17" t="str">
+        <v>MARACUJA AZEDO</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>75</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+      <c r="G17">
+        <v>7.5</v>
+      </c>
+      <c r="H17">
+        <v>11.85</v>
+      </c>
+      <c r="I17">
+        <v>0.58</v>
+      </c>
+      <c r="J17">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>28</v>
+      </c>
+      <c r="B18" t="str">
+        <v>MELANCIA</v>
+      </c>
+      <c r="C18">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>35</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>12</v>
+      </c>
+      <c r="G18">
+        <v>35</v>
+      </c>
+      <c r="H18">
+        <v>55.3</v>
+      </c>
+      <c r="I18">
+        <v>0.58</v>
+      </c>
+      <c r="J18">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>29</v>
+      </c>
+      <c r="B19" t="str">
+        <v>MELAO AMARELO</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>65</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>21</v>
+      </c>
+      <c r="G19">
+        <v>9.29</v>
+      </c>
+      <c r="H19">
+        <v>14.67</v>
+      </c>
+      <c r="I19">
+        <v>0.58</v>
+      </c>
+      <c r="J19">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>29</v>
+      </c>
+      <c r="B20" t="str">
+        <v>MELAO PELE-DE-SAPO</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>30</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="H20">
+        <v>9.48</v>
+      </c>
+      <c r="I20">
+        <v>0.58</v>
+      </c>
+      <c r="J20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>36</v>
+      </c>
+      <c r="B21" t="str">
+        <v>MORANGO</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>25</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <v>6.25</v>
+      </c>
+      <c r="H21">
+        <v>9.88</v>
+      </c>
+      <c r="I21">
+        <v>0.5808</v>
+      </c>
+      <c r="J21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>37</v>
+      </c>
+      <c r="B22" t="str">
+        <v>NECTARINA</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>90</v>
+      </c>
+      <c r="E22">
+        <v>9</v>
+      </c>
+      <c r="F22">
+        <v>9</v>
+      </c>
+      <c r="G22">
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <v>15.8</v>
+      </c>
+      <c r="I22">
+        <v>0.58</v>
+      </c>
+      <c r="J22">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>39</v>
+      </c>
+      <c r="B23" t="str">
+        <v>PERA WILLIAMS</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>108</v>
+      </c>
+      <c r="E23">
+        <v>18</v>
+      </c>
+      <c r="F23">
+        <v>18</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+      <c r="H23">
+        <v>9.48</v>
+      </c>
+      <c r="I23">
+        <v>0.58</v>
+      </c>
+      <c r="J23">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>40</v>
+      </c>
+      <c r="B24" t="str">
+        <v>PESSEGO</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>150</v>
+      </c>
+      <c r="E24">
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>24</v>
+      </c>
+      <c r="G24">
+        <v>12.5</v>
+      </c>
+      <c r="H24">
+        <v>19.75</v>
+      </c>
+      <c r="I24">
+        <v>0.58</v>
+      </c>
+      <c r="J24">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>2281</v>
+      </c>
+      <c r="B25" t="str">
+        <v>UVA VERDE SEM SEMENTE</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>90</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>20</v>
+      </c>
+      <c r="G25">
+        <v>9</v>
+      </c>
+      <c r="H25">
+        <v>14.22</v>
+      </c>
+      <c r="I25">
+        <v>0.58</v>
+      </c>
+      <c r="J25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>51</v>
+      </c>
+      <c r="B26" t="str">
+        <v>AMENDOIM</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>85</v>
+      </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
+      <c r="F26">
+        <v>10</v>
+      </c>
+      <c r="G26">
+        <v>8.5</v>
+      </c>
+      <c r="H26">
+        <v>13.43</v>
+      </c>
+      <c r="I26">
+        <v>0.58</v>
+      </c>
+      <c r="J26">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>56</v>
+      </c>
+      <c r="B27" t="str">
+        <v>BETERRABA</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>50</v>
+      </c>
+      <c r="E27">
+        <v>16</v>
+      </c>
+      <c r="F27">
+        <v>16</v>
+      </c>
+      <c r="G27">
+        <v>3.13</v>
+      </c>
+      <c r="H27">
+        <v>4.94</v>
+      </c>
+      <c r="I27">
+        <v>0.58</v>
+      </c>
+      <c r="J27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>60</v>
+      </c>
+      <c r="B28" t="str">
+        <v>CEBOLA NACIONAL</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>45</v>
+      </c>
+      <c r="E28">
+        <v>20</v>
+      </c>
+      <c r="F28">
+        <v>40</v>
+      </c>
+      <c r="G28">
+        <v>2.25</v>
+      </c>
+      <c r="H28">
+        <v>3.55</v>
+      </c>
+      <c r="I28">
+        <v>0.5778</v>
+      </c>
+      <c r="J28">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>67</v>
+      </c>
+      <c r="B29" t="str">
+        <v>MILHO VERDE</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>35</v>
+      </c>
+      <c r="E29">
+        <v>10</v>
+      </c>
+      <c r="F29">
+        <v>10</v>
+      </c>
+      <c r="G29">
+        <v>3.5</v>
+      </c>
+      <c r="H29">
+        <v>5.53</v>
+      </c>
+      <c r="I29">
+        <v>0.58</v>
+      </c>
+      <c r="J29">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>76</v>
+      </c>
+      <c r="B30" t="str">
+        <v>TOMATE PIZZADORO</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>120</v>
+      </c>
+      <c r="E30">
+        <v>16</v>
+      </c>
+      <c r="F30">
+        <v>16</v>
+      </c>
+      <c r="G30">
+        <v>7.5</v>
+      </c>
+      <c r="H30">
+        <v>11.85</v>
+      </c>
+      <c r="I30">
+        <v>0.58</v>
+      </c>
+      <c r="J30">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>78</v>
+      </c>
+      <c r="B31" t="str">
+        <v>AGRIAO</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>40</v>
+      </c>
+      <c r="E31">
+        <v>14</v>
+      </c>
+      <c r="F31">
+        <v>14</v>
+      </c>
+      <c r="G31">
+        <v>2.86</v>
+      </c>
+      <c r="H31">
+        <v>4.52</v>
+      </c>
+      <c r="I31">
+        <v>0.5804</v>
+      </c>
+      <c r="J31">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32" t="str">
+        <v>ALFACE CRESPA</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>40</v>
+      </c>
+      <c r="E32">
+        <v>18</v>
+      </c>
+      <c r="F32">
+        <v>36</v>
+      </c>
+      <c r="G32">
+        <v>2.22</v>
+      </c>
+      <c r="H32">
+        <v>3.51</v>
+      </c>
+      <c r="I32">
+        <v>0.58</v>
+      </c>
+      <c r="J32">
         <v>80</v>
       </c>
-      <c r="E9">
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>79</v>
+      </c>
+      <c r="B33" t="str">
+        <v>ALFACE LISA</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
         <v>18</v>
       </c>
-      <c r="F9">
-        <v>36</v>
-      </c>
-      <c r="G9">
-        <v>4.44</v>
-      </c>
-      <c r="H9">
-        <v>7.02</v>
-      </c>
-      <c r="I9">
-        <v>0.58</v>
-      </c>
-      <c r="J9">
-        <v>160</v>
+      <c r="E33">
+        <v>18</v>
+      </c>
+      <c r="F33">
+        <v>18</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1.58</v>
+      </c>
+      <c r="I33">
+        <v>0.58</v>
+      </c>
+      <c r="J33">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>79</v>
+      </c>
+      <c r="B34" t="str">
+        <v>ALHO PORO</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>30</v>
+      </c>
+      <c r="E34">
+        <v>12</v>
+      </c>
+      <c r="F34">
+        <v>12</v>
+      </c>
+      <c r="G34">
+        <v>2.5</v>
+      </c>
+      <c r="H34">
+        <v>3.95</v>
+      </c>
+      <c r="I34">
+        <v>0.58</v>
+      </c>
+      <c r="J34">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>82</v>
+      </c>
+      <c r="B35" t="str">
+        <v>BROCOLIS NINJA</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>8</v>
+      </c>
+      <c r="G35">
+        <v>8</v>
+      </c>
+      <c r="H35">
+        <v>12.64</v>
+      </c>
+      <c r="I35">
+        <v>0.58</v>
+      </c>
+      <c r="J35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>82</v>
+      </c>
+      <c r="B36" t="str">
+        <v>CEBOLINHA</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <v>8</v>
+      </c>
+      <c r="H36">
+        <v>12.64</v>
+      </c>
+      <c r="I36">
+        <v>0.58</v>
+      </c>
+      <c r="J36">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>84</v>
+      </c>
+      <c r="B37" t="str">
+        <v>COENTRO</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>20</v>
+      </c>
+      <c r="E37">
+        <v>6</v>
+      </c>
+      <c r="F37">
+        <v>30</v>
+      </c>
+      <c r="G37">
+        <v>3.33</v>
+      </c>
+      <c r="H37">
+        <v>5.27</v>
+      </c>
+      <c r="I37">
+        <v>0.58</v>
+      </c>
+      <c r="J37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>86</v>
+      </c>
+      <c r="B38" t="str">
+        <v>COUVE MANTEIGA</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>45</v>
+      </c>
+      <c r="E38">
+        <v>24</v>
+      </c>
+      <c r="F38">
+        <v>24</v>
+      </c>
+      <c r="G38">
+        <v>1.88</v>
+      </c>
+      <c r="H38">
+        <v>2.96</v>
+      </c>
+      <c r="I38">
+        <v>0.5798</v>
+      </c>
+      <c r="J38">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>88</v>
+      </c>
+      <c r="B39" t="str">
+        <v>RUCULA</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>50</v>
+      </c>
+      <c r="E39">
+        <v>14</v>
+      </c>
+      <c r="F39">
+        <v>14</v>
+      </c>
+      <c r="G39">
+        <v>3.57</v>
+      </c>
+      <c r="H39">
+        <v>5.64</v>
+      </c>
+      <c r="I39">
+        <v>0.58</v>
+      </c>
+      <c r="J39">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>91</v>
+      </c>
+      <c r="B40" t="str">
+        <v>SALSA</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>20</v>
+      </c>
+      <c r="E40">
+        <v>19</v>
+      </c>
+      <c r="F40">
+        <v>38</v>
+      </c>
+      <c r="G40">
+        <v>1.05</v>
+      </c>
+      <c r="H40">
+        <v>1.66</v>
+      </c>
+      <c r="I40">
+        <v>0.58</v>
+      </c>
+      <c r="J40">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J40"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[FIX](cors): The url was set in CORS and hide in environment variables
</commit_message>
<xml_diff>
--- a/src/data/relatorios/xlsx/relatorio.xlsx
+++ b/src/data/relatorios/xlsx/relatorio.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Relatório Compra 15-03-2025" sheetId="1" r:id="rId1"/>
+    <sheet name="Relatório Compra 16-03-2025" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -442,193 +442,353 @@
         <v>LIMAO TAITI</v>
       </c>
       <c r="C2">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>260</v>
+        <v>45</v>
       </c>
       <c r="E2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F2">
-        <v>1404</v>
+        <v>88</v>
       </c>
       <c r="G2">
-        <v>4.81</v>
+        <v>1.02</v>
       </c>
       <c r="H2">
-        <v>7.61</v>
+        <v>1.62</v>
       </c>
       <c r="I2">
         <v>0.58</v>
       </c>
       <c r="J2">
-        <v>6760</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B3" t="str">
-        <v>MANGA PALMER</v>
+        <v>BANANA NANICA</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="E3">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F3">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G3">
-        <v>5.29</v>
+        <v>2.5</v>
       </c>
       <c r="H3">
-        <v>8.36</v>
+        <v>3.95</v>
       </c>
       <c r="I3">
         <v>0.58</v>
       </c>
       <c r="J3">
-        <v>180</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="str">
-        <v>BANANA NANICA</v>
+        <v>BANANA PRATA</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="E4">
         <v>20</v>
       </c>
       <c r="F4">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>2.25</v>
       </c>
       <c r="H4">
-        <v>6.32</v>
+        <v>3.55</v>
       </c>
       <c r="I4">
-        <v>0.58</v>
+        <v>0.5788</v>
       </c>
       <c r="J4">
-        <v>160</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B5" t="str">
-        <v>BERINJELA</v>
+        <v>MAMAO PAPAIA</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F5">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>15.3</v>
+        <v>3.16</v>
       </c>
       <c r="I5">
-        <v>0.7</v>
+        <v>0.58</v>
       </c>
       <c r="J5">
-        <v>180</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="B6" t="str">
-        <v>LIMAO TAITI</v>
+        <v>BATATA LAVADA</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="E6">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F6">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G6">
-        <v>1.82</v>
+        <v>3.6</v>
       </c>
       <c r="H6">
-        <v>2.87</v>
+        <v>5.87</v>
       </c>
       <c r="I6">
-        <v>0.58</v>
+        <v>0.63</v>
       </c>
       <c r="J6">
-        <v>80</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B7" t="str">
-        <v>UVA RUBI</v>
+        <v>CAQUI CHOCOLATE</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>13.04</v>
+      </c>
+      <c r="I7">
+        <v>0.63</v>
+      </c>
+      <c r="J7">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>28</v>
+      </c>
+      <c r="B8" t="str">
+        <v>MELANCIA</v>
+      </c>
+      <c r="C8">
         <v>10</v>
       </c>
-      <c r="G7">
+      <c r="D8">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>30</v>
+      </c>
+      <c r="H8">
+        <v>48.9</v>
+      </c>
+      <c r="I8">
+        <v>0.63</v>
+      </c>
+      <c r="J8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>62</v>
+      </c>
+      <c r="B9" t="str">
+        <v>CHUCHU</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>45</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>4.5</v>
+      </c>
+      <c r="H9">
+        <v>7.33</v>
+      </c>
+      <c r="I9">
+        <v>0.63</v>
+      </c>
+      <c r="J9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="str">
+        <v>LARANJA PERA</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+      <c r="E10">
+        <v>22</v>
+      </c>
+      <c r="F10">
+        <v>44</v>
+      </c>
+      <c r="G10">
+        <v>2.27</v>
+      </c>
+      <c r="H10">
+        <v>3.7</v>
+      </c>
+      <c r="I10">
+        <v>0.63</v>
+      </c>
+      <c r="J10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="str">
+        <v>MACA FUJI</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>90</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>40</v>
+      </c>
+      <c r="G11">
+        <v>4.5</v>
+      </c>
+      <c r="H11">
+        <v>8.1</v>
+      </c>
+      <c r="I11">
+        <v>0.8</v>
+      </c>
+      <c r="J11">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
         <v>4</v>
       </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <v>0.5</v>
-      </c>
-      <c r="J7">
-        <v>40</v>
+      <c r="B12" t="str">
+        <v>ALFACE CRESPA</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>30</v>
+      </c>
+      <c r="E12">
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>54</v>
+      </c>
+      <c r="G12">
+        <v>1.67</v>
+      </c>
+      <c r="H12">
+        <v>2.63</v>
+      </c>
+      <c r="I12">
+        <v>0.58</v>
+      </c>
+      <c r="J12">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[FEAT]: Api url was set.
</commit_message>
<xml_diff>
--- a/src/data/relatorios/xlsx/relatorio.xlsx
+++ b/src/data/relatorios/xlsx/relatorio.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Relatório Compra 16-03-2025" sheetId="1" r:id="rId1"/>
+    <sheet name="Relatório Compra 21-05-2025" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -436,63 +436,63 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B2" t="str">
-        <v>LIMAO TAITI</v>
+        <v>ABACATE MANTEIGA</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="F2">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="G2">
-        <v>1.02</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>1.62</v>
+        <v>1.57</v>
       </c>
       <c r="I2">
-        <v>0.58</v>
+        <v>0.57</v>
       </c>
       <c r="J2">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B3" t="str">
-        <v>BANANA NANICA</v>
+        <v>LIMAO TAITI</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F3">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G3">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>3.95</v>
+        <v>1.5</v>
       </c>
       <c r="I3">
-        <v>0.58</v>
+        <v>0.5</v>
       </c>
       <c r="J3">
         <v>100</v>
@@ -500,295 +500,71 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="B4" t="str">
-        <v>BANANA PRATA</v>
+        <v>ABOBORA SECA</v>
       </c>
       <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
         <v>1</v>
       </c>
-      <c r="D4">
-        <v>45</v>
-      </c>
-      <c r="E4">
-        <v>20</v>
-      </c>
-      <c r="F4">
-        <v>20</v>
-      </c>
-      <c r="G4">
-        <v>2.25</v>
-      </c>
       <c r="H4">
-        <v>3.55</v>
+        <v>1.5</v>
       </c>
       <c r="I4">
-        <v>0.5788</v>
+        <v>0.5</v>
       </c>
       <c r="J4">
-        <v>45</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B5" t="str">
-        <v>MAMAO PAPAIA</v>
+        <v>BANANA MACA</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F5">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>3.16</v>
+        <v>1.48</v>
       </c>
       <c r="I5">
-        <v>0.58</v>
+        <v>0.48</v>
       </c>
       <c r="J5">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>53</v>
-      </c>
-      <c r="B6" t="str">
-        <v>BATATA LAVADA</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>90</v>
-      </c>
-      <c r="E6">
-        <v>25</v>
-      </c>
-      <c r="F6">
-        <v>50</v>
-      </c>
-      <c r="G6">
-        <v>3.6</v>
-      </c>
-      <c r="H6">
-        <v>5.87</v>
-      </c>
-      <c r="I6">
-        <v>0.63</v>
-      </c>
-      <c r="J6">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>13</v>
-      </c>
-      <c r="B7" t="str">
-        <v>CAQUI CHOCOLATE</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>80</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>20</v>
-      </c>
-      <c r="G7">
-        <v>8</v>
-      </c>
-      <c r="H7">
-        <v>13.04</v>
-      </c>
-      <c r="I7">
-        <v>0.63</v>
-      </c>
-      <c r="J7">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>28</v>
-      </c>
-      <c r="B8" t="str">
-        <v>MELANCIA</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>30</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <v>30</v>
-      </c>
-      <c r="H8">
-        <v>48.9</v>
-      </c>
-      <c r="I8">
-        <v>0.63</v>
-      </c>
-      <c r="J8">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>62</v>
-      </c>
-      <c r="B9" t="str">
-        <v>CHUCHU</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>45</v>
-      </c>
-      <c r="E9">
-        <v>10</v>
-      </c>
-      <c r="F9">
-        <v>20</v>
-      </c>
-      <c r="G9">
-        <v>4.5</v>
-      </c>
-      <c r="H9">
-        <v>7.33</v>
-      </c>
-      <c r="I9">
-        <v>0.63</v>
-      </c>
-      <c r="J9">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="str">
-        <v>LARANJA PERA</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>50</v>
-      </c>
-      <c r="E10">
-        <v>22</v>
-      </c>
-      <c r="F10">
-        <v>44</v>
-      </c>
-      <c r="G10">
-        <v>2.27</v>
-      </c>
-      <c r="H10">
-        <v>3.7</v>
-      </c>
-      <c r="I10">
-        <v>0.63</v>
-      </c>
-      <c r="J10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11" t="str">
-        <v>MACA FUJI</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>90</v>
-      </c>
-      <c r="E11">
-        <v>20</v>
-      </c>
-      <c r="F11">
-        <v>40</v>
-      </c>
-      <c r="G11">
-        <v>4.5</v>
-      </c>
-      <c r="H11">
-        <v>8.1</v>
-      </c>
-      <c r="I11">
-        <v>0.8</v>
-      </c>
-      <c r="J11">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12">
-        <v>4</v>
-      </c>
-      <c r="B12" t="str">
-        <v>ALFACE CRESPA</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>30</v>
-      </c>
-      <c r="E12">
-        <v>18</v>
-      </c>
-      <c r="F12">
-        <v>54</v>
-      </c>
-      <c r="G12">
-        <v>1.67</v>
-      </c>
-      <c r="H12">
-        <v>2.63</v>
-      </c>
-      <c r="I12">
-        <v>0.58</v>
-      </c>
-      <c r="J12">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>